<commit_message>
feat(IPT): Calculations for the first block completed.
</commit_message>
<xml_diff>
--- a/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/IPT/EE734_IPT_Design_Report_24_UPI.xlsx
+++ b/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/IPT/EE734_IPT_Design_Report_24_UPI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoa-my.sharepoint.com/personal/skim281_uoa_auckland_ac_nz/Documents/Teaching/Electeng 734/2024/EE734 Design Report Student Package 2024/IPT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\ELECTENG 734\Wirlessly-Powered-RC-Car\Implementation\EE734 Design Report Student Package 2024\EE734 Design Report Student Package 2024\IPT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="6_{D0018338-B9B7-48E8-873D-943073820194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D2424F1-6CF3-4676-B55C-41605E6004C6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A240A8-BD77-45B5-B95E-AB68EED2F3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operating Conditions" sheetId="1" r:id="rId1"/>
@@ -1505,7 +1505,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1650,15 +1650,24 @@
       <c r="A17" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="B17" s="9"/>
+      <c r="B17" s="9">
+        <f>B7*1.1</f>
+        <v>1.2869999999999999</v>
+      </c>
       <c r="C17" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="9"/>
+      <c r="D17" s="9">
+        <f>B6/D16</f>
+        <v>1</v>
+      </c>
       <c r="E17" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="F17" s="9"/>
+      <c r="F17" s="9">
+        <f>B6/F16</f>
+        <v>0.6</v>
+      </c>
       <c r="G17" s="16" t="s">
         <v>81</v>
       </c>
@@ -1667,15 +1676,23 @@
       <c r="A18" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="9"/>
+      <c r="B18" s="9">
+        <f>B17*B16</f>
+        <v>12.87</v>
+      </c>
       <c r="C18" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="9"/>
+      <c r="D18" s="9">
+        <f>D17*D16</f>
+        <v>15</v>
+      </c>
       <c r="E18" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="F18" s="9"/>
+      <c r="F18" s="9">
+        <v>15</v>
+      </c>
       <c r="G18" s="16" t="s">
         <v>82</v>
       </c>
@@ -1684,15 +1701,24 @@
       <c r="A19" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="9"/>
+      <c r="B19" s="9">
+        <f>B17^2 *B16</f>
+        <v>16.563689999999998</v>
+      </c>
       <c r="C19" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="9"/>
+      <c r="D19" s="9">
+        <f>D18^2/D16</f>
+        <v>15</v>
+      </c>
       <c r="E19" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="F19" s="9"/>
+      <c r="F19" s="9">
+        <f>F18^2/F16</f>
+        <v>9</v>
+      </c>
       <c r="G19" s="16" t="s">
         <v>83</v>
       </c>
@@ -1701,15 +1727,22 @@
       <c r="A20" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="9"/>
+      <c r="B20" s="9">
+        <v>0</v>
+      </c>
       <c r="C20" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="9"/>
+      <c r="D20" s="9">
+        <f>22.3</f>
+        <v>22.3</v>
+      </c>
       <c r="E20" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="9"/>
+      <c r="F20" s="9">
+        <v>53.38</v>
+      </c>
       <c r="G20" s="16" t="s">
         <v>12</v>
       </c>
@@ -1718,7 +1751,10 @@
       <c r="A21" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="B21" s="53"/>
+      <c r="B21" s="53">
+        <f>B19/($B$7*$B$8)</f>
+        <v>1.9883426966292135</v>
+      </c>
       <c r="C21" s="54" t="s">
         <v>86</v>
       </c>
@@ -1735,15 +1771,24 @@
       <c r="A22" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="B22" s="17"/>
+      <c r="B22" s="17">
+        <f>B19/($B$7*$B$8)</f>
+        <v>1.9883426966292135</v>
+      </c>
       <c r="C22" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="17"/>
+      <c r="D22" s="17">
+        <f>D19/($B$7*$B$8)</f>
+        <v>1.8006338231057335</v>
+      </c>
       <c r="E22" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="F22" s="17"/>
+      <c r="F22" s="17">
+        <f>F19/($B$7*$B$8)</f>
+        <v>1.0803802938634401</v>
+      </c>
       <c r="G22" s="19" t="s">
         <v>87</v>
       </c>
@@ -3323,14 +3368,14 @@
       </c>
       <c r="D26" s="28">
         <f>'Operating Conditions'!D20</f>
-        <v>0</v>
+        <v>22.3</v>
       </c>
       <c r="E26" s="26" t="s">
         <v>11</v>
       </c>
       <c r="F26" s="28">
         <f>'Operating Conditions'!F20</f>
-        <v>0</v>
+        <v>53.38</v>
       </c>
       <c r="G26" s="27" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
feat(IPT): Partial completion of compensator values
</commit_message>
<xml_diff>
--- a/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/IPT/EE734_IPT_Design_Report_24_UPI.xlsx
+++ b/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/IPT/EE734_IPT_Design_Report_24_UPI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\ELECTENG 734\Wirlessly-Powered-RC-Car\Implementation\EE734 Design Report Student Package 2024\EE734 Design Report Student Package 2024\IPT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A240A8-BD77-45B5-B95E-AB68EED2F3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185025D3-AB88-44B4-89FD-E4215B0554C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operating Conditions" sheetId="1" r:id="rId1"/>
@@ -1504,8 +1504,8 @@
   </sheetPr>
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1758,11 +1758,15 @@
       <c r="C21" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="53"/>
+      <c r="D21" s="53">
+        <v>2.3199999999999998</v>
+      </c>
       <c r="E21" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="F21" s="53"/>
+      <c r="F21" s="53">
+        <v>2.3199999999999998</v>
+      </c>
       <c r="G21" s="55" t="s">
         <v>86</v>
       </c>
@@ -1815,7 +1819,9 @@
       <c r="A28" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="B28" s="12"/>
+      <c r="B28" s="12">
+        <v>0.67139000000000004</v>
+      </c>
       <c r="C28" s="14" t="s">
         <v>91</v>
       </c>
@@ -1876,8 +1882,8 @@
   </sheetPr>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2249,7 +2255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="F47" sqref="F47:F48"/>
     </sheetView>
   </sheetViews>
@@ -2659,7 +2665,7 @@
   </sheetPr>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -3169,7 +3175,7 @@
   </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
feat(IPT): Partial completion of Cdc calculations.
</commit_message>
<xml_diff>
--- a/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/IPT/EE734_IPT_Design_Report_24_UPI.xlsx
+++ b/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/IPT/EE734_IPT_Design_Report_24_UPI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\ELECTENG 734\Wirlessly-Powered-RC-Car\Implementation\EE734 Design Report Student Package 2024\EE734 Design Report Student Package 2024\IPT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185025D3-AB88-44B4-89FD-E4215B0554C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBDAB90-86DB-4B35-BA91-5E6CCBCA64DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="750" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operating Conditions" sheetId="1" r:id="rId1"/>
@@ -1504,8 +1504,8 @@
   </sheetPr>
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1882,8 +1882,8 @@
   </sheetPr>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1984,7 +1984,9 @@
       <c r="A15" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="29"/>
+      <c r="B15" s="29">
+        <v>324.88600000000002</v>
+      </c>
       <c r="C15" s="35" t="s">
         <v>98</v>
       </c>
@@ -2039,7 +2041,9 @@
       <c r="A23" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="42"/>
+      <c r="B23" s="42">
+        <v>25</v>
+      </c>
       <c r="C23" s="33" t="s">
         <v>8</v>
       </c>
@@ -2049,6 +2053,9 @@
       <c r="A24" s="39" t="s">
         <v>28</v>
       </c>
+      <c r="B24">
+        <v>470</v>
+      </c>
       <c r="C24" s="27" t="s">
         <v>29</v>
       </c>
@@ -2057,7 +2064,9 @@
       <c r="A25" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="42"/>
+      <c r="B25" s="42">
+        <v>130</v>
+      </c>
       <c r="C25" s="33" t="s">
         <v>31</v>
       </c>
@@ -2066,7 +2075,9 @@
       <c r="A26" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="43"/>
+      <c r="B26" s="43">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="C26" s="35" t="s">
         <v>9</v>
       </c>
@@ -2255,7 +2266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="F47" sqref="F47:F48"/>
     </sheetView>
   </sheetViews>
@@ -2665,7 +2676,7 @@
   </sheetPr>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -3175,7 +3186,7 @@
   </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
feat(IPT): Pick-up converter design part II - Capacitor and controller calculations.
</commit_message>
<xml_diff>
--- a/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/IPT/EE734_IPT_Design_Report_24_UPI.xlsx
+++ b/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/IPT/EE734_IPT_Design_Report_24_UPI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\ELECTENG 734\Wirlessly-Powered-RC-Car\Implementation\EE734 Design Report Student Package 2024\EE734 Design Report Student Package 2024\IPT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBDAB90-86DB-4B35-BA91-5E6CCBCA64DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCE65D8-D3D5-4F6E-ABA0-B73DCF50D14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="750" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="750" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operating Conditions" sheetId="1" r:id="rId1"/>
@@ -1505,7 +1505,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1830,7 +1830,9 @@
       <c r="A29" s="51" t="s">
         <v>93</v>
       </c>
-      <c r="B29" s="9"/>
+      <c r="B29" s="9">
+        <v>16.5</v>
+      </c>
       <c r="C29" s="20" t="s">
         <v>94</v>
       </c>
@@ -1882,8 +1884,8 @@
   </sheetPr>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2139,15 +2141,21 @@
       <c r="A33" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="B33" s="61"/>
+      <c r="B33" s="61">
+        <v>0</v>
+      </c>
       <c r="C33" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="D33" s="61"/>
+      <c r="D33" s="61">
+        <v>479.09</v>
+      </c>
       <c r="E33" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="F33" s="61"/>
+      <c r="F33" s="61">
+        <v>688.08799999999997</v>
+      </c>
       <c r="G33" s="63" t="s">
         <v>102</v>
       </c>
@@ -2156,15 +2164,21 @@
       <c r="A34" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="25"/>
+      <c r="B34" s="25">
+        <v>0</v>
+      </c>
       <c r="C34" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="D34" s="25"/>
+      <c r="D34" s="25">
+        <v>0.75660000000000005</v>
+      </c>
       <c r="E34" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="F34" s="25"/>
+      <c r="F34" s="25">
+        <v>0.7823</v>
+      </c>
       <c r="G34" s="27" t="s">
         <v>103</v>
       </c>
@@ -2173,15 +2187,21 @@
       <c r="A35" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="34"/>
+      <c r="B35" s="34">
+        <v>0</v>
+      </c>
       <c r="C35" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="D35" s="34"/>
+      <c r="D35" s="34">
+        <v>74.400000000000006</v>
+      </c>
       <c r="E35" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="34">
+        <v>79.56</v>
+      </c>
       <c r="G35" s="31" t="s">
         <v>104</v>
       </c>
@@ -2231,7 +2251,9 @@
       <c r="A43" s="48" t="s">
         <v>153</v>
       </c>
-      <c r="B43" s="28"/>
+      <c r="B43" s="28">
+        <v>10</v>
+      </c>
       <c r="C43" s="33" t="s">
         <v>75</v>
       </c>
@@ -2240,7 +2262,9 @@
       <c r="A44" s="66" t="s">
         <v>154</v>
       </c>
-      <c r="B44" s="69"/>
+      <c r="B44" s="69">
+        <v>14.33</v>
+      </c>
       <c r="C44" s="33" t="s">
         <v>105</v>
       </c>
@@ -2249,7 +2273,9 @@
       <c r="A45" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="B45" s="29"/>
+      <c r="B45" s="29">
+        <v>214.95</v>
+      </c>
       <c r="C45" s="35" t="s">
         <v>106</v>
       </c>
@@ -2266,7 +2292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
       <selection activeCell="F47" sqref="F47:F48"/>
     </sheetView>
   </sheetViews>
@@ -2676,7 +2702,7 @@
   </sheetPr>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat(IPT): Partial completion of FET and diode calculations.
</commit_message>
<xml_diff>
--- a/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/IPT/EE734_IPT_Design_Report_24_UPI.xlsx
+++ b/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/IPT/EE734_IPT_Design_Report_24_UPI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\ELECTENG 734\Wirlessly-Powered-RC-Car\Implementation\EE734 Design Report Student Package 2024\EE734 Design Report Student Package 2024\IPT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UniversityOfAuckland\ELECTENG 734\Wirlessly-Powered-RC-Car\Implementation\EE734 Design Report Student Package 2024\EE734 Design Report Student Package 2024\IPT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCE65D8-D3D5-4F6E-ABA0-B73DCF50D14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE0646B-A3AC-4977-986C-263F61A0CF0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="750" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operating Conditions" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="181">
   <si>
     <t>Specifications</t>
   </si>
@@ -580,6 +580,12 @@
   </si>
   <si>
     <t>IPP052N06L3</t>
+  </si>
+  <si>
+    <t>Diodes Inc.</t>
+  </si>
+  <si>
+    <t>SBR4040CTFP</t>
   </si>
 </sst>
 </file>
@@ -651,7 +657,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -672,6 +678,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1111,20 +1123,19 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="2" applyBorder="1"/>
@@ -1151,7 +1162,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="2" applyBorder="1"/>
@@ -1160,8 +1170,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="2" applyFont="1" applyBorder="1"/>
@@ -1174,10 +1182,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="2" applyFont="1" applyBorder="1"/>
@@ -1189,13 +1195,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1205,18 +1207,27 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -1504,8 +1515,8 @@
   </sheetPr>
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1526,68 +1537,68 @@
     </row>
     <row r="4" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="70">
+      <c r="B6" s="63">
         <v>15</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="20" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="71">
+      <c r="B7" s="64">
         <v>1.17</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="19" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="47" t="s">
         <v>151</v>
       </c>
-      <c r="B8" s="71">
+      <c r="B8" s="64">
         <v>7.12</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="19" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="47" t="s">
         <v>152</v>
       </c>
-      <c r="B9" s="71">
+      <c r="B9" s="64">
         <v>25</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="B10" s="72">
+      <c r="B10" s="65">
         <v>38.4</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="21" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1601,199 +1612,199 @@
     </row>
     <row r="14" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="50" t="s">
+      <c r="A16" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="73">
+      <c r="B16" s="63">
         <v>10</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="73">
+      <c r="D16" s="63">
         <v>15</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="73">
+      <c r="F16" s="63">
         <v>25</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="51" t="s">
+      <c r="A17" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="8">
         <f>B7*1.1</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="8">
         <f>B6/D16</f>
         <v>1</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="8">
         <f>B6/F16</f>
         <v>0.6</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="G17" s="15" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="51" t="s">
+      <c r="A18" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="8">
         <f>B17*B16</f>
         <v>12.87</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="8">
         <f>D17*D16</f>
         <v>15</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="8">
         <v>15</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="G18" s="15" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="51" t="s">
+      <c r="A19" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="8">
         <f>B17^2 *B16</f>
         <v>16.563689999999998</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="8">
         <f>D18^2/D16</f>
         <v>15</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="8">
         <f>F18^2/F16</f>
         <v>9</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="15" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="8">
         <v>0</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="8">
         <f>22.3</f>
         <v>22.3</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="8">
         <v>53.38</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="15" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="56" t="s">
+      <c r="A21" s="52" t="s">
         <v>84</v>
       </c>
-      <c r="B21" s="53">
+      <c r="B21" s="49">
         <f>B19/($B$7*$B$8)</f>
         <v>1.9883426966292135</v>
       </c>
-      <c r="C21" s="54" t="s">
+      <c r="C21" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="53">
+      <c r="D21" s="49">
         <v>2.3199999999999998</v>
       </c>
-      <c r="E21" s="54" t="s">
+      <c r="E21" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="F21" s="53">
+      <c r="F21" s="49">
         <v>2.3199999999999998</v>
       </c>
-      <c r="G21" s="55" t="s">
+      <c r="G21" s="51" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="52" t="s">
+      <c r="A22" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="B22" s="17">
+      <c r="B22" s="16">
         <f>B19/($B$7*$B$8)</f>
         <v>1.9883426966292135</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="16">
         <f>D19/($B$7*$B$8)</f>
         <v>1.8006338231057335</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="F22" s="17">
+      <c r="F22" s="16">
         <f>F19/($B$7*$B$8)</f>
         <v>1.0803802938634401</v>
       </c>
-      <c r="G22" s="19" t="s">
+      <c r="G22" s="18" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1805,66 +1816,65 @@
     </row>
     <row r="26" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="B28" s="12">
+      <c r="B28" s="11">
         <v>0.67139000000000004</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="13" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="B29" s="9">
+      <c r="B29" s="8">
         <v>16.5</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="19" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="52" t="s">
+      <c r="A30" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="19" t="s">
+      <c r="B30" s="85">
+        <v>2.6669999999999998</v>
+      </c>
+      <c r="C30" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
       <c r="B31" s="5"/>
       <c r="C31" s="4"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
       <c r="B32" s="5"/>
       <c r="C32" s="4"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="4"/>
       <c r="F33" s="5"/>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
     </row>
   </sheetData>
@@ -1884,8 +1894,8 @@
   </sheetPr>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1908,59 +1918,59 @@
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="74">
+      <c r="B6" s="66">
         <v>1000</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="23" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="75">
+      <c r="B7" s="67">
         <f>'Operating Conditions'!B6</f>
         <v>15</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="32" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="75">
+      <c r="B8" s="67">
         <f>'Operating Conditions'!B7*1.1</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="32" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="76">
+      <c r="B9" s="68">
         <v>1</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="34" t="s">
         <v>176</v>
       </c>
     </row>
@@ -1972,36 +1982,34 @@
     </row>
     <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="49" t="s">
+      <c r="A15" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="29">
+      <c r="B15" s="79">
         <v>324.88600000000002</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="34" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="60"/>
-      <c r="B16" s="58"/>
-      <c r="C16" s="59"/>
+      <c r="A16" s="54"/>
+      <c r="B16" s="6"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="60"/>
-      <c r="B17" s="58"/>
-      <c r="C17" s="59"/>
+      <c r="A17" s="54"/>
+      <c r="B17" s="6"/>
     </row>
     <row r="18" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -2010,77 +2018,77 @@
     </row>
     <row r="19" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="77" t="s">
+      <c r="B21" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="32"/>
+      <c r="C21" s="31"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="78" t="s">
+      <c r="B22" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="F22" s="8"/>
+      <c r="C22" s="32"/>
+      <c r="F22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="42">
+      <c r="B23" s="40">
         <v>25</v>
       </c>
-      <c r="C23" s="33" t="s">
+      <c r="C23" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="8"/>
+      <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="37" t="s">
         <v>28</v>
       </c>
       <c r="B24">
         <v>470</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="26" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="42">
+      <c r="B25" s="40">
         <v>130</v>
       </c>
-      <c r="C25" s="33" t="s">
+      <c r="C25" s="32" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="40" t="s">
+      <c r="A26" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="43">
+      <c r="B26" s="41">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C26" s="35" t="s">
+      <c r="C26" s="34" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2092,117 +2100,117 @@
     </row>
     <row r="30" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F31" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="G31" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="38" t="s">
+      <c r="A32" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="79">
+      <c r="B32" s="71">
         <v>10</v>
       </c>
-      <c r="C32" s="23" t="s">
+      <c r="C32" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D32" s="79">
+      <c r="D32" s="71">
         <v>15</v>
       </c>
-      <c r="E32" s="23" t="s">
+      <c r="E32" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F32" s="79">
+      <c r="F32" s="71">
         <v>25</v>
       </c>
-      <c r="G32" s="24" t="s">
+      <c r="G32" s="23" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="64" t="s">
+      <c r="A33" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="B33" s="61">
+      <c r="B33" s="55">
         <v>0</v>
       </c>
-      <c r="C33" s="62" t="s">
+      <c r="C33" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="D33" s="61">
+      <c r="D33" s="80">
         <v>479.09</v>
       </c>
-      <c r="E33" s="62" t="s">
+      <c r="E33" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="F33" s="61">
+      <c r="F33" s="80">
         <v>688.08799999999997</v>
       </c>
-      <c r="G33" s="63" t="s">
+      <c r="G33" s="57" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="39" t="s">
+      <c r="A34" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="25">
+      <c r="B34" s="24">
         <v>0</v>
       </c>
-      <c r="C34" s="26" t="s">
+      <c r="C34" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="D34" s="25">
+      <c r="D34" s="81">
         <v>0.75660000000000005</v>
       </c>
-      <c r="E34" s="26" t="s">
+      <c r="E34" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="F34" s="25">
+      <c r="F34" s="81">
         <v>0.7823</v>
       </c>
-      <c r="G34" s="27" t="s">
+      <c r="G34" s="26" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="40" t="s">
+      <c r="A35" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="34">
+      <c r="B35" s="33">
         <v>0</v>
       </c>
-      <c r="C35" s="30" t="s">
+      <c r="C35" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="D35" s="34">
+      <c r="D35" s="82">
         <v>74.400000000000006</v>
       </c>
-      <c r="E35" s="30" t="s">
+      <c r="E35" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="F35" s="34">
+      <c r="F35" s="82">
         <v>79.56</v>
       </c>
-      <c r="G35" s="31" t="s">
+      <c r="G35" s="30" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2214,69 +2222,69 @@
     </row>
     <row r="39" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="40" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="57" t="s">
+      <c r="A41" s="53" t="s">
         <v>100</v>
       </c>
-      <c r="B41" s="67">
+      <c r="B41" s="61">
         <v>4</v>
       </c>
-      <c r="C41" s="32" t="s">
+      <c r="C41" s="31" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="64" t="s">
+      <c r="A42" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="B42" s="68">
+      <c r="B42" s="62">
         <f>'Operating Conditions'!B6</f>
         <v>15</v>
       </c>
-      <c r="C42" s="65" t="s">
+      <c r="C42" s="59" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="48" t="s">
+      <c r="A43" s="44" t="s">
         <v>153</v>
       </c>
-      <c r="B43" s="28">
+      <c r="B43" s="27">
         <v>10</v>
       </c>
-      <c r="C43" s="33" t="s">
+      <c r="C43" s="32" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="66" t="s">
+      <c r="A44" s="60" t="s">
         <v>154</v>
       </c>
-      <c r="B44" s="69">
+      <c r="B44" s="78">
         <v>14.33</v>
       </c>
-      <c r="C44" s="33" t="s">
+      <c r="C44" s="32" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="49" t="s">
+      <c r="A45" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="B45" s="29">
+      <c r="B45" s="79">
         <v>214.95</v>
       </c>
-      <c r="C45" s="35" t="s">
+      <c r="C45" s="34" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2292,8 +2300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47:F48"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2314,66 +2322,63 @@
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="B6" s="75">
+      <c r="B6" s="67">
         <f>'Operating Conditions'!B7*1.1</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="32" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="B7" s="75">
+      <c r="B7" s="67">
         <f>'Operating Conditions'!B10</f>
         <v>38.4</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="32" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="B8" s="75">
+      <c r="B8" s="67">
         <v>0.25</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="32" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="B9" s="76">
+      <c r="B9" s="68">
         <v>5</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="34" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-    </row>
     <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>141</v>
@@ -2381,107 +2386,107 @@
     </row>
     <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="B15" s="83" t="s">
+      <c r="B15" s="74" t="s">
         <v>117</v>
       </c>
-      <c r="C15" s="24"/>
+      <c r="C15" s="23"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="B16" s="78">
+      <c r="B16" s="70">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="32" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="37" t="s">
         <v>119</v>
       </c>
-      <c r="B17" s="75">
+      <c r="B17" s="67">
         <v>28.3</v>
       </c>
-      <c r="C17" s="33" t="s">
+      <c r="C17" s="32" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="B18" s="75">
+      <c r="B18" s="67">
         <v>36</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="32" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="B19" s="75">
+      <c r="B19" s="67">
         <v>31.5</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="32" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="B20" s="84">
+      <c r="B20" s="75">
         <f>1.8*10^-8</f>
         <v>1.8000000000000002E-8</v>
       </c>
-      <c r="C20" s="33" t="s">
+      <c r="C20" s="32" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="B21" s="84">
+      <c r="B21" s="75">
         <f>4*PI()*10^-7</f>
         <v>1.2566370614359173E-6</v>
       </c>
-      <c r="C21" s="33" t="s">
+      <c r="C21" s="32" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="B22" s="76">
+      <c r="B22" s="68">
         <v>0.7</v>
       </c>
-      <c r="C22" s="37"/>
+      <c r="C22" s="34"/>
     </row>
     <row r="23" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="81"/>
+      <c r="A24" s="72"/>
       <c r="B24" s="5"/>
     </row>
     <row r="25" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -2494,42 +2499,42 @@
       <c r="B26" s="5"/>
     </row>
     <row r="27" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="57" t="s">
+      <c r="A28" s="53" t="s">
         <v>130</v>
       </c>
-      <c r="B28" s="74">
+      <c r="B28" s="66">
         <v>200</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="31" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="B29" s="76">
+      <c r="B29" s="68">
         <v>0.56000000000000005</v>
       </c>
-      <c r="C29" s="35" t="s">
+      <c r="C29" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="F29" s="8"/>
+      <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="7"/>
-      <c r="F30" s="8"/>
+      <c r="B30" s="6"/>
+      <c r="F30" s="7"/>
     </row>
     <row r="32" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
@@ -2538,68 +2543,74 @@
     </row>
     <row r="33" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="64" t="s">
+      <c r="A35" s="58" t="s">
         <v>133</v>
       </c>
-      <c r="B35" s="85"/>
-      <c r="C35" s="65" t="s">
+      <c r="B35" s="76">
+        <v>63</v>
+      </c>
+      <c r="C35" s="59" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="B36" s="86"/>
-      <c r="C36" s="33" t="s">
+      <c r="B36" s="27">
+        <v>0.29865999999999998</v>
+      </c>
+      <c r="C36" s="32" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="48" t="s">
+      <c r="A37" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="B37" s="87"/>
-      <c r="C37" s="33" t="s">
+      <c r="B37" s="77">
+        <v>0.24629999999999999</v>
+      </c>
+      <c r="C37" s="32" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="48" t="s">
+      <c r="A38" s="44" t="s">
         <v>149</v>
       </c>
       <c r="B38" s="86"/>
-      <c r="C38" s="33" t="s">
+      <c r="C38" s="32" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="39" t="s">
+      <c r="A39" s="37" t="s">
         <v>136</v>
       </c>
       <c r="B39" s="86"/>
-      <c r="C39" s="33" t="s">
+      <c r="C39" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="E39" s="82"/>
+      <c r="E39" s="73"/>
     </row>
     <row r="40" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="40" t="s">
+      <c r="A40" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="B40" s="88"/>
-      <c r="C40" s="35" t="s">
+      <c r="B40" s="82"/>
+      <c r="C40" s="34" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2611,82 +2622,82 @@
     </row>
     <row r="44" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="D45" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E45" s="11" t="s">
+      <c r="E45" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F45" s="11" t="s">
+      <c r="F45" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G45" s="11" t="s">
+      <c r="G45" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="38" t="s">
+      <c r="A46" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B46" s="79">
+      <c r="B46" s="71">
         <v>10</v>
       </c>
-      <c r="C46" s="23" t="s">
+      <c r="C46" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D46" s="79">
+      <c r="D46" s="71">
         <v>15</v>
       </c>
-      <c r="E46" s="23" t="s">
+      <c r="E46" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F46" s="79">
+      <c r="F46" s="71">
         <v>25</v>
       </c>
-      <c r="G46" s="24" t="s">
+      <c r="G46" s="23" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="39" t="s">
+      <c r="A47" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="B47" s="25"/>
-      <c r="C47" s="26" t="s">
+      <c r="B47" s="81"/>
+      <c r="C47" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D47" s="25"/>
-      <c r="E47" s="26" t="s">
+      <c r="D47" s="81"/>
+      <c r="E47" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F47" s="25"/>
-      <c r="G47" s="27" t="s">
+      <c r="F47" s="81"/>
+      <c r="G47" s="26" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="39" t="s">
+      <c r="A48" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="B48" s="28"/>
-      <c r="C48" s="26" t="s">
+      <c r="B48" s="86"/>
+      <c r="C48" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="D48" s="28"/>
-      <c r="E48" s="26" t="s">
+      <c r="D48" s="86"/>
+      <c r="E48" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="F48" s="28"/>
-      <c r="G48" s="27" t="s">
+      <c r="F48" s="86"/>
+      <c r="G48" s="26" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2702,8 +2713,8 @@
   </sheetPr>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2724,48 +2735,48 @@
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="74">
+      <c r="B6" s="66">
         <f>'Operating Conditions'!B6</f>
         <v>15</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="75">
+      <c r="B7" s="67">
         <f>'Operating Conditions'!B7*1.1</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="32" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="76">
+      <c r="B8" s="68">
         <v>30</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="34" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2777,103 +2788,119 @@
     </row>
     <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="39" t="s">
         <v>177</v>
       </c>
-      <c r="C14" s="32"/>
+      <c r="C14" s="31"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="C15" s="33"/>
+      <c r="C15" s="32"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="42"/>
-      <c r="C16" s="33" t="s">
+      <c r="B16" s="40">
+        <v>60</v>
+      </c>
+      <c r="C16" s="32" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="27" t="s">
+      <c r="B17" s="40">
+        <v>80</v>
+      </c>
+      <c r="C17" s="26" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="42"/>
-      <c r="C18" s="33" t="s">
+      <c r="B18" s="40">
+        <v>5</v>
+      </c>
+      <c r="C18" s="32" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="42"/>
-      <c r="C19" s="33" t="s">
+      <c r="B19" s="40">
+        <v>12</v>
+      </c>
+      <c r="C19" s="32" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="42"/>
-      <c r="C20" s="33" t="s">
+      <c r="B20" s="40">
+        <v>47</v>
+      </c>
+      <c r="C20" s="32" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="42"/>
-      <c r="C21" s="33" t="s">
+      <c r="B21" s="83">
+        <v>4.5</v>
+      </c>
+      <c r="C21" s="32" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="42"/>
-      <c r="C22" s="33" t="s">
+      <c r="B22" s="83">
+        <v>8</v>
+      </c>
+      <c r="C22" s="32" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="35" t="s">
+      <c r="B23" s="84">
+        <v>62</v>
+      </c>
+      <c r="C23" s="34" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2885,51 +2912,52 @@
     </row>
     <row r="26" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="74">
+      <c r="B28" s="66">
         <f>B6</f>
         <v>15</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="31" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="75">
+      <c r="B29" s="67">
         <v>0.1</v>
       </c>
-      <c r="C29" s="33" t="s">
+      <c r="C29" s="32" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="29"/>
-      <c r="C30" s="35" t="s">
+      <c r="B30" s="28">
+        <v>150</v>
+      </c>
+      <c r="C30" s="34" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="7"/>
+      <c r="B31" s="6"/>
     </row>
     <row r="33" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
@@ -2938,235 +2966,256 @@
     </row>
     <row r="34" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="E35" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F35" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="G35" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="38" t="s">
+      <c r="A36" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B36" s="80">
+      <c r="B36" s="66">
         <v>10</v>
       </c>
-      <c r="C36" s="23" t="s">
+      <c r="C36" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="79">
+      <c r="D36" s="71">
         <v>15</v>
       </c>
-      <c r="E36" s="23" t="s">
+      <c r="E36" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F36" s="79">
+      <c r="F36" s="71">
         <v>25</v>
       </c>
-      <c r="G36" s="24" t="s">
+      <c r="G36" s="23" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="48" t="s">
+      <c r="A37" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="B37" s="28"/>
-      <c r="C37" s="26" t="s">
+      <c r="B37" s="27">
+        <f>'Capacitor &amp; Controller'!B33</f>
+        <v>0</v>
+      </c>
+      <c r="C37" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="D37" s="25"/>
-      <c r="E37" s="26" t="s">
+      <c r="D37" s="27">
+        <f>'Capacitor &amp; Controller'!D33</f>
+        <v>479.09</v>
+      </c>
+      <c r="E37" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="F37" s="25"/>
-      <c r="G37" s="27" t="s">
+      <c r="F37" s="27">
+        <f>'Capacitor &amp; Controller'!F33</f>
+        <v>688.08799999999997</v>
+      </c>
+      <c r="G37" s="26" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="39" t="s">
+      <c r="A38" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="28"/>
-      <c r="C38" s="26" t="s">
+      <c r="B38" s="27">
+        <v>0</v>
+      </c>
+      <c r="C38" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D38" s="28"/>
-      <c r="E38" s="26" t="s">
+      <c r="D38" s="27">
+        <f>Switch!B7*SQRT('Operating Conditions'!D20/100)</f>
+        <v>0.6077584117064937</v>
+      </c>
+      <c r="E38" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F38" s="28"/>
-      <c r="G38" s="27" t="s">
+      <c r="F38" s="27">
+        <f>B7*SQRT('Operating Conditions'!F20/100)</f>
+        <v>0.9403030214776511</v>
+      </c>
+      <c r="G38" s="26" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="39" t="s">
+      <c r="A39" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="B39" s="28"/>
-      <c r="C39" s="26" t="s">
+      <c r="B39" s="27">
+        <v>0</v>
+      </c>
+      <c r="C39" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="D39" s="28"/>
-      <c r="E39" s="26" t="s">
+      <c r="D39" s="86"/>
+      <c r="E39" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="F39" s="28"/>
-      <c r="G39" s="27" t="s">
+      <c r="F39" s="86"/>
+      <c r="G39" s="26" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="39" t="s">
+      <c r="A40" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="B40" s="28"/>
-      <c r="C40" s="26" t="s">
+      <c r="B40" s="27">
+        <v>0</v>
+      </c>
+      <c r="C40" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="D40" s="28"/>
-      <c r="E40" s="26" t="s">
+      <c r="D40" s="86"/>
+      <c r="E40" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="F40" s="28"/>
-      <c r="G40" s="27" t="s">
+      <c r="F40" s="86"/>
+      <c r="G40" s="26" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="48" t="s">
+      <c r="A41" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="B41" s="28"/>
-      <c r="C41" s="26" t="s">
+      <c r="B41" s="86"/>
+      <c r="C41" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="D41" s="28"/>
-      <c r="E41" s="26" t="s">
+      <c r="D41" s="86"/>
+      <c r="E41" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="F41" s="28"/>
-      <c r="G41" s="27" t="s">
+      <c r="F41" s="86"/>
+      <c r="G41" s="26" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="28"/>
-      <c r="C42" s="26" t="s">
+      <c r="B42" s="86"/>
+      <c r="C42" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="D42" s="28"/>
-      <c r="E42" s="26" t="s">
+      <c r="D42" s="86"/>
+      <c r="E42" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F42" s="28"/>
-      <c r="G42" s="27" t="s">
+      <c r="F42" s="86"/>
+      <c r="G42" s="26" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="B43" s="28"/>
-      <c r="C43" s="26" t="s">
+      <c r="B43" s="86"/>
+      <c r="C43" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="D43" s="28"/>
-      <c r="E43" s="26" t="s">
+      <c r="D43" s="86"/>
+      <c r="E43" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="F43" s="28"/>
-      <c r="G43" s="27" t="s">
+      <c r="F43" s="86"/>
+      <c r="G43" s="26" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="39" t="s">
+      <c r="A44" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="B44" s="28"/>
-      <c r="C44" s="26" t="s">
+      <c r="B44" s="86"/>
+      <c r="C44" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="D44" s="28"/>
-      <c r="E44" s="26" t="s">
+      <c r="D44" s="86"/>
+      <c r="E44" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="F44" s="28"/>
-      <c r="G44" s="27" t="s">
+      <c r="F44" s="86"/>
+      <c r="G44" s="26" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="39" t="s">
+      <c r="A45" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="B45" s="28"/>
-      <c r="C45" s="26" t="s">
+      <c r="B45" s="86"/>
+      <c r="C45" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="D45" s="28"/>
-      <c r="E45" s="26" t="s">
+      <c r="D45" s="86"/>
+      <c r="E45" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="F45" s="28"/>
-      <c r="G45" s="26" t="s">
+      <c r="F45" s="86"/>
+      <c r="G45" s="25" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="39" t="s">
+      <c r="A46" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="B46" s="28"/>
-      <c r="C46" s="30" t="s">
+      <c r="B46" s="86"/>
+      <c r="C46" s="29" t="s">
         <v>170</v>
       </c>
-      <c r="D46" s="28"/>
-      <c r="E46" s="30" t="s">
+      <c r="D46" s="86"/>
+      <c r="E46" s="29" t="s">
         <v>170</v>
       </c>
-      <c r="F46" s="28"/>
-      <c r="G46" s="30" t="s">
+      <c r="F46" s="86"/>
+      <c r="G46" s="29" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="40" t="s">
+      <c r="A47" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B47" s="29"/>
-      <c r="C47" s="30" t="s">
+      <c r="B47" s="79"/>
+      <c r="C47" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="D47" s="29"/>
-      <c r="E47" s="30" t="s">
+      <c r="D47" s="79"/>
+      <c r="E47" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="F47" s="29"/>
-      <c r="G47" s="30" t="s">
+      <c r="F47" s="79"/>
+      <c r="G47" s="29" t="s">
         <v>146</v>
       </c>
     </row>
@@ -3178,22 +3227,22 @@
     </row>
     <row r="51" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="52" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="11" t="s">
+      <c r="A52" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="11" t="s">
+      <c r="B52" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="C52" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="47" t="s">
+      <c r="A53" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="B53" s="45"/>
-      <c r="C53" s="46" t="s">
+      <c r="B53" s="87"/>
+      <c r="C53" s="42" t="s">
         <v>171</v>
       </c>
     </row>
@@ -3212,7 +3261,9 @@
   </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3232,48 +3283,48 @@
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="74">
+      <c r="B6" s="66">
         <f>'Operating Conditions'!B6</f>
         <v>15</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="75">
+      <c r="B7" s="67">
         <f>'Capacitor &amp; Controller'!B8</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="32" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="76">
+      <c r="B8" s="68">
         <v>30</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="34" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3285,63 +3336,75 @@
     </row>
     <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="32"/>
+      <c r="B14" s="39" t="s">
+        <v>179</v>
+      </c>
+      <c r="C14" s="31"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="33"/>
+      <c r="B15" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="C15" s="32"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="B16" s="42"/>
-      <c r="C16" s="33" t="s">
+      <c r="B16" s="40">
+        <v>40</v>
+      </c>
+      <c r="C16" s="32" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="27" t="s">
+      <c r="B17" s="83">
+        <v>40</v>
+      </c>
+      <c r="C17" s="26" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="42"/>
-      <c r="C18" s="33" t="s">
+      <c r="B18" s="40">
+        <v>0.53</v>
+      </c>
+      <c r="C18" s="32" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="35" t="s">
+      <c r="B19" s="84">
+        <v>4</v>
+      </c>
+      <c r="C19" s="34" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3353,142 +3416,142 @@
     </row>
     <row r="23" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G24" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="80">
+      <c r="B25" s="66">
         <v>10</v>
       </c>
-      <c r="C25" s="23" t="s">
+      <c r="C25" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="79">
+      <c r="D25" s="71">
         <v>15</v>
       </c>
-      <c r="E25" s="23" t="s">
+      <c r="E25" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="79">
+      <c r="F25" s="71">
         <v>25</v>
       </c>
-      <c r="G25" s="24" t="s">
+      <c r="G25" s="23" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="28">
+      <c r="B26" s="27">
         <f>'Operating Conditions'!B20</f>
         <v>0</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="28">
+      <c r="D26" s="27">
         <f>'Operating Conditions'!D20</f>
         <v>22.3</v>
       </c>
-      <c r="E26" s="26" t="s">
+      <c r="E26" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="28">
+      <c r="F26" s="27">
         <f>'Operating Conditions'!F20</f>
         <v>53.38</v>
       </c>
-      <c r="G26" s="27" t="s">
+      <c r="G26" s="26" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="26" t="s">
+      <c r="B27" s="86"/>
+      <c r="C27" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="D27" s="28"/>
-      <c r="E27" s="26" t="s">
+      <c r="D27" s="86"/>
+      <c r="E27" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="F27" s="28"/>
-      <c r="G27" s="26" t="s">
+      <c r="F27" s="86"/>
+      <c r="G27" s="25" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="26" t="s">
+      <c r="B28" s="86"/>
+      <c r="C28" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="D28" s="28"/>
-      <c r="E28" s="26" t="s">
+      <c r="D28" s="86"/>
+      <c r="E28" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="F28" s="28"/>
-      <c r="G28" s="26" t="s">
+      <c r="F28" s="86"/>
+      <c r="G28" s="25" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="26" t="s">
+      <c r="B29" s="86"/>
+      <c r="C29" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="D29" s="28"/>
-      <c r="E29" s="26" t="s">
+      <c r="D29" s="86"/>
+      <c r="E29" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="F29" s="28"/>
-      <c r="G29" s="26" t="s">
+      <c r="F29" s="86"/>
+      <c r="G29" s="25" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="29"/>
-      <c r="C30" s="30" t="s">
+      <c r="B30" s="79"/>
+      <c r="C30" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="D30" s="29"/>
-      <c r="E30" s="30" t="s">
+      <c r="D30" s="79"/>
+      <c r="E30" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="F30" s="29"/>
-      <c r="G30" s="30" t="s">
+      <c r="F30" s="79"/>
+      <c r="G30" s="29" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3500,22 +3563,22 @@
     </row>
     <row r="34" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="47" t="s">
+      <c r="A36" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="45"/>
-      <c r="C36" s="46" t="s">
+      <c r="B36" s="87"/>
+      <c r="C36" s="42" t="s">
         <v>174</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(IPT): Completed all calculations for IPT implementation. TO DO: Populate remaining equations.
</commit_message>
<xml_diff>
--- a/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/IPT/EE734_IPT_Design_Report_24_UPI.xlsx
+++ b/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/IPT/EE734_IPT_Design_Report_24_UPI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UniversityOfAuckland\ELECTENG 734\Wirlessly-Powered-RC-Car\Implementation\EE734 Design Report Student Package 2024\EE734 Design Report Student Package 2024\IPT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE0646B-A3AC-4977-986C-263F61A0CF0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27A95FC-6D2D-4A8D-88EE-7B7F9BDAC494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="750" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operating Conditions" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="183">
   <si>
     <t>Specifications</t>
   </si>
@@ -582,10 +582,16 @@
     <t>IPP052N06L3</t>
   </si>
   <si>
-    <t>Diodes Inc.</t>
-  </si>
-  <si>
-    <t>SBR4040CTFP</t>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>VS-MBR1045-M3</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Approximation assuming similar RthJA to MOSFET</t>
   </si>
 </sst>
 </file>
@@ -688,7 +694,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -1117,13 +1123,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1220,14 +1252,28 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -1515,8 +1561,8 @@
   </sheetPr>
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1852,7 +1898,7 @@
       <c r="A30" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="B30" s="85">
+      <c r="B30" s="83">
         <v>2.6669999999999998</v>
       </c>
       <c r="C30" s="18" t="s">
@@ -1894,8 +1940,8 @@
   </sheetPr>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1996,7 +2042,7 @@
       <c r="A15" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="79">
+      <c r="B15" s="84">
         <v>324.88600000000002</v>
       </c>
       <c r="C15" s="34" t="s">
@@ -2155,13 +2201,13 @@
       <c r="C33" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="D33" s="80">
+      <c r="D33" s="85">
         <v>479.09</v>
       </c>
       <c r="E33" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="F33" s="80">
+      <c r="F33" s="85">
         <v>688.08799999999997</v>
       </c>
       <c r="G33" s="57" t="s">
@@ -2178,14 +2224,14 @@
       <c r="C34" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="D34" s="81">
-        <v>0.75660000000000005</v>
+      <c r="D34" s="80">
+        <v>0.28727999999999998</v>
       </c>
       <c r="E34" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="F34" s="81">
-        <v>0.7823</v>
+      <c r="F34" s="80">
+        <v>0.41413</v>
       </c>
       <c r="G34" s="26" t="s">
         <v>103</v>
@@ -2201,14 +2247,14 @@
       <c r="C35" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="D35" s="82">
-        <v>74.400000000000006</v>
+      <c r="D35" s="81">
+        <v>10.728999999999999</v>
       </c>
       <c r="E35" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="F35" s="82">
-        <v>79.56</v>
+      <c r="F35" s="81">
+        <v>22.295000000000002</v>
       </c>
       <c r="G35" s="30" t="s">
         <v>104</v>
@@ -2259,7 +2305,7 @@
       <c r="A43" s="44" t="s">
         <v>153</v>
       </c>
-      <c r="B43" s="27">
+      <c r="B43" s="82">
         <v>10</v>
       </c>
       <c r="C43" s="32" t="s">
@@ -2300,8 +2346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2590,7 +2636,9 @@
       <c r="A38" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="B38" s="86"/>
+      <c r="B38" s="86">
+        <v>22.167000000000002</v>
+      </c>
       <c r="C38" s="32" t="s">
         <v>142</v>
       </c>
@@ -2599,7 +2647,9 @@
       <c r="A39" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="B39" s="86"/>
+      <c r="B39" s="86">
+        <v>5.2374999999999998</v>
+      </c>
       <c r="C39" s="32" t="s">
         <v>163</v>
       </c>
@@ -2609,7 +2659,9 @@
       <c r="A40" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="B40" s="82"/>
+      <c r="B40" s="87">
+        <v>145.03</v>
+      </c>
       <c r="C40" s="34" t="s">
         <v>164</v>
       </c>
@@ -2671,15 +2723,21 @@
       <c r="A47" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="B47" s="81"/>
+      <c r="B47" s="88">
+        <v>1.29</v>
+      </c>
       <c r="C47" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D47" s="81"/>
+      <c r="D47" s="88">
+        <v>1.29</v>
+      </c>
       <c r="E47" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F47" s="81"/>
+      <c r="F47" s="88">
+        <v>1.29</v>
+      </c>
       <c r="G47" s="26" t="s">
         <v>9</v>
       </c>
@@ -2688,15 +2746,21 @@
       <c r="A48" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="B48" s="86"/>
+      <c r="B48" s="86">
+        <v>241.34</v>
+      </c>
       <c r="C48" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="D48" s="86"/>
+      <c r="D48" s="86">
+        <v>241.34</v>
+      </c>
       <c r="E48" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="F48" s="86"/>
+      <c r="F48" s="86">
+        <v>241.34</v>
+      </c>
       <c r="G48" s="26" t="s">
         <v>165</v>
       </c>
@@ -2713,7 +2777,7 @@
   </sheetPr>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
@@ -2875,7 +2939,7 @@
       <c r="A21" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="83">
+      <c r="B21" s="89">
         <v>4.5</v>
       </c>
       <c r="C21" s="32" t="s">
@@ -2886,8 +2950,8 @@
       <c r="A22" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="83">
-        <v>8</v>
+      <c r="B22" s="89">
+        <v>5</v>
       </c>
       <c r="C22" s="32" t="s">
         <v>31</v>
@@ -2897,7 +2961,7 @@
       <c r="A23" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="84">
+      <c r="B23" s="90">
         <v>62</v>
       </c>
       <c r="C23" s="34" t="s">
@@ -3072,11 +3136,17 @@
       <c r="C39" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="D39" s="86"/>
+      <c r="D39" s="86">
+        <f>$B$7-((1*8*'Capacitor &amp; Controller'!$B$15*10^-6*D37)/2)</f>
+        <v>0.66440146503999986</v>
+      </c>
       <c r="E39" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="F39" s="86"/>
+      <c r="F39" s="86">
+        <f>$B$7-((1*8*'Capacitor &amp; Controller'!$B$15*10^-6*F37)/2)</f>
+        <v>0.39279936812799987</v>
+      </c>
       <c r="G39" s="26" t="s">
         <v>167</v>
       </c>
@@ -3091,11 +3161,17 @@
       <c r="C40" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="D40" s="86"/>
+      <c r="D40" s="86">
+        <f>$B$7+((1*8*'Capacitor &amp; Controller'!$B$15*10^-6*D37)/2)</f>
+        <v>1.90959853496</v>
+      </c>
       <c r="E40" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="F40" s="86"/>
+      <c r="F40" s="86">
+        <f>$B$7+((1*8*'Capacitor &amp; Controller'!$B$15*10^-6*F37)/2)</f>
+        <v>2.1812006318720001</v>
+      </c>
       <c r="G40" s="26" t="s">
         <v>167</v>
       </c>
@@ -3104,15 +3180,24 @@
       <c r="A41" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="B41" s="86"/>
+      <c r="B41" s="86">
+        <f>($B$6-$B$22*10^-3*B39)*(($B$30*$B$20*10^-12)/($B$28-$B$21))*10^9</f>
+        <v>10.071428571428571</v>
+      </c>
       <c r="C41" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="D41" s="86"/>
+      <c r="D41" s="86">
+        <f>($B$6-$B$22*10^-3*D39)*(($B$30*$B$20*10^-12)/($B$28-$B$21))*10^9</f>
+        <v>10.069198080795937</v>
+      </c>
       <c r="E41" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="F41" s="86"/>
+      <c r="F41" s="86">
+        <f>($B$6-$B$22*10^-3*F39)*(($B$30*$B$20*10^-12)/($B$28-$B$21))*10^9</f>
+        <v>10.070109887835573</v>
+      </c>
       <c r="G41" s="26" t="s">
         <v>168</v>
       </c>
@@ -3121,15 +3206,24 @@
       <c r="A42" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="86"/>
+      <c r="B42" s="86">
+        <f>($B$6-$B$22*10^-3*$D$40)*(($B$30*$B$20*10^-12)/($B$21))*10^9</f>
+        <v>23.485041478142811</v>
+      </c>
       <c r="C42" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="D42" s="86"/>
+      <c r="D42" s="86">
+        <f>($B$6-$B$22*10^-3*$D$40)*(($B$30*$B$20*10^-12)/($B$21))*10^9</f>
+        <v>23.485041478142811</v>
+      </c>
       <c r="E42" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F42" s="86"/>
+      <c r="F42" s="86">
+        <f>($B$6-$B$22*10^-3*$D$40)*(($B$30*$B$20*10^-12)/($B$21))*10^9</f>
+        <v>23.485041478142811</v>
+      </c>
       <c r="G42" s="26" t="s">
         <v>143</v>
       </c>
@@ -3138,15 +3232,24 @@
       <c r="A43" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="B43" s="86"/>
+      <c r="B43" s="86">
+        <f>$B$18+$B$41</f>
+        <v>15.071428571428571</v>
+      </c>
       <c r="C43" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="D43" s="86"/>
+      <c r="D43" s="86">
+        <f>$B$18+$B$41</f>
+        <v>15.071428571428571</v>
+      </c>
       <c r="E43" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="F43" s="86"/>
+      <c r="F43" s="86">
+        <f>$B$18+$B$41</f>
+        <v>15.071428571428571</v>
+      </c>
       <c r="G43" s="26" t="s">
         <v>144</v>
       </c>
@@ -3155,15 +3258,24 @@
       <c r="A44" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="B44" s="86"/>
+      <c r="B44" s="86">
+        <f>$B$19+$B$42</f>
+        <v>35.485041478142811</v>
+      </c>
       <c r="C44" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="D44" s="86"/>
+      <c r="D44" s="86">
+        <f>$B$19+$B$42</f>
+        <v>35.485041478142811</v>
+      </c>
       <c r="E44" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="F44" s="86"/>
+      <c r="F44" s="86">
+        <f>$B$19+$B$42</f>
+        <v>35.485041478142811</v>
+      </c>
       <c r="G44" s="26" t="s">
         <v>145</v>
       </c>
@@ -3172,15 +3284,23 @@
       <c r="A45" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="B45" s="86"/>
+      <c r="B45" s="86">
+        <v>0</v>
+      </c>
       <c r="C45" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="D45" s="86"/>
+      <c r="D45" s="86">
+        <f>((D37*$B$6)/2)*(D39*D43*10^-9+D40*D44*10^-9)*1000</f>
+        <v>0.27946156589776133</v>
+      </c>
       <c r="E45" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="F45" s="86"/>
+      <c r="F45" s="86">
+        <f>((F37*$B$6)/2)*(F39*F43*10^-9+F40*F44*10^-9)*1000</f>
+        <v>0.42998641059912607</v>
+      </c>
       <c r="G45" s="25" t="s">
         <v>169</v>
       </c>
@@ -3189,15 +3309,23 @@
       <c r="A46" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="B46" s="86"/>
+      <c r="B46" s="86">
+        <v>0</v>
+      </c>
       <c r="C46" s="29" t="s">
         <v>170</v>
       </c>
-      <c r="D46" s="86"/>
+      <c r="D46" s="86">
+        <f>D$38^2*$B$22</f>
+        <v>1.8468514349999996</v>
+      </c>
       <c r="E46" s="29" t="s">
         <v>170</v>
       </c>
-      <c r="F46" s="86"/>
+      <c r="F46" s="86">
+        <f>F$38^2*$B$22</f>
+        <v>4.4208488610000005</v>
+      </c>
       <c r="G46" s="29" t="s">
         <v>170</v>
       </c>
@@ -3206,15 +3334,23 @@
       <c r="A47" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B47" s="79"/>
+      <c r="B47" s="84">
+        <v>0</v>
+      </c>
       <c r="C47" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="D47" s="79"/>
+      <c r="D47" s="84">
+        <f>SUM(D45:D46)</f>
+        <v>2.1263130008977611</v>
+      </c>
       <c r="E47" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="F47" s="79"/>
+      <c r="F47" s="84">
+        <f>SUM(F45:F46)</f>
+        <v>4.8508352715991263</v>
+      </c>
       <c r="G47" s="29" t="s">
         <v>146</v>
       </c>
@@ -3241,7 +3377,10 @@
       <c r="A53" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="B53" s="87"/>
+      <c r="B53" s="91">
+        <f>B8+B23*F47*10^-3</f>
+        <v>30.300751786839147</v>
+      </c>
       <c r="C53" s="42" t="s">
         <v>171</v>
       </c>
@@ -3261,8 +3400,8 @@
   </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3359,17 +3498,17 @@
       <c r="A15" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="92" t="s">
         <v>180</v>
       </c>
-      <c r="C15" s="32"/>
+      <c r="C15" s="93"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
         <v>69</v>
       </c>
       <c r="B16" s="40">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C16" s="32" t="s">
         <v>8</v>
@@ -3379,8 +3518,8 @@
       <c r="A17" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="83">
-        <v>40</v>
+      <c r="B17" s="89">
+        <v>10</v>
       </c>
       <c r="C17" s="26" t="s">
         <v>9</v>
@@ -3391,7 +3530,7 @@
         <v>71</v>
       </c>
       <c r="B18" s="40">
-        <v>0.53</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="C18" s="32" t="s">
         <v>8</v>
@@ -3401,8 +3540,8 @@
       <c r="A19" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="84">
-        <v>4</v>
+      <c r="B19" s="94" t="s">
+        <v>181</v>
       </c>
       <c r="C19" s="34" t="s">
         <v>65</v>
@@ -3491,15 +3630,24 @@
       <c r="A27" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="86"/>
+      <c r="B27" s="86">
+        <f>B7</f>
+        <v>1.2869999999999999</v>
+      </c>
       <c r="C27" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="D27" s="86"/>
+      <c r="D27" s="86">
+        <f>(1-D26/100)*$B$7</f>
+        <v>0.99999899999999997</v>
+      </c>
       <c r="E27" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="F27" s="86"/>
+      <c r="F27" s="86">
+        <f>(1-F26/100)*$B$7</f>
+        <v>0.59999939999999985</v>
+      </c>
       <c r="G27" s="25" t="s">
         <v>172</v>
       </c>
@@ -3508,15 +3656,24 @@
       <c r="A28" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="86"/>
+      <c r="B28" s="86">
+        <f>(1-B26/100)*$B$18*$B$7</f>
+        <v>0.73358999999999985</v>
+      </c>
       <c r="C28" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="D28" s="86"/>
+      <c r="D28" s="86">
+        <f>(1-D26/100)*$B$18*$B$7</f>
+        <v>0.56999942999999986</v>
+      </c>
       <c r="E28" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="F28" s="86"/>
+      <c r="F28" s="86">
+        <f>(1-F26/100)*$B$18*$B$7</f>
+        <v>0.34199965799999993</v>
+      </c>
       <c r="G28" s="25" t="s">
         <v>173</v>
       </c>
@@ -3525,15 +3682,21 @@
       <c r="A29" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="B29" s="86"/>
+      <c r="B29" s="86">
+        <v>0</v>
+      </c>
       <c r="C29" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="D29" s="86"/>
+      <c r="D29" s="86">
+        <v>0</v>
+      </c>
       <c r="E29" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="F29" s="86"/>
+      <c r="F29" s="86">
+        <v>0</v>
+      </c>
       <c r="G29" s="25" t="s">
         <v>147</v>
       </c>
@@ -3542,27 +3705,36 @@
       <c r="A30" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="79"/>
+      <c r="B30" s="84">
+        <f>SUM(B28:B29)</f>
+        <v>0.73358999999999985</v>
+      </c>
       <c r="C30" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="D30" s="79"/>
+      <c r="D30" s="84">
+        <f>SUM(D28:D29)</f>
+        <v>0.56999942999999986</v>
+      </c>
       <c r="E30" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="F30" s="79"/>
+      <c r="F30" s="84">
+        <f>SUM(F28:F29)</f>
+        <v>0.34199965799999993</v>
+      </c>
       <c r="G30" s="29" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>2</v>
       </c>
@@ -3573,17 +3745,28 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="87"/>
+      <c r="B36" s="91">
+        <v>75</v>
+      </c>
       <c r="C36" s="42" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="D36" s="95" t="s">
+        <v>182</v>
+      </c>
+      <c r="E36" s="95"/>
+      <c r="F36" s="95"/>
+      <c r="G36" s="95"/>
+    </row>
+    <row r="37" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B15:C15"/>
+  </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="96" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
feat(IPT): Completed IPT section.
</commit_message>
<xml_diff>
--- a/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/IPT/EE734_IPT_Design_Report_24_UPI.xlsx
+++ b/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/IPT/EE734_IPT_Design_Report_24_UPI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UniversityOfAuckland\ELECTENG 734\Wirlessly-Powered-RC-Car\Implementation\EE734 Design Report Student Package 2024\EE734 Design Report Student Package 2024\IPT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LeonD\Documents\ELECTENG 734\Wirlessly-Powered-RC-Car\Implementation\EE734 Design Report Student Package 2024\EE734 Design Report Student Package 2024\IPT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27A95FC-6D2D-4A8D-88EE-7B7F9BDAC494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB01257-1A34-4581-827D-7AE68ADF65A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="750" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" tabRatio="750" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operating Conditions" sheetId="1" r:id="rId1"/>
@@ -1155,7 +1155,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1248,32 +1248,24 @@
     <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -1562,27 +1554,27 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.75" customWidth="1"/>
-    <col min="2" max="7" width="11.875" customWidth="1"/>
+    <col min="2" max="7" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
@@ -1593,7 +1585,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A6" s="46" t="s">
         <v>76</v>
       </c>
@@ -1604,7 +1596,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="47" t="s">
         <v>77</v>
       </c>
@@ -1615,7 +1607,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="47" t="s">
         <v>151</v>
       </c>
@@ -1626,7 +1618,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="47" t="s">
         <v>152</v>
       </c>
@@ -1637,7 +1629,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="48" t="s">
         <v>90</v>
       </c>
@@ -1648,16 +1640,16 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
     </row>
-    <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="15" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="10" t="s">
         <v>2</v>
       </c>
@@ -1680,7 +1672,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A16" s="46" t="s">
         <v>5</v>
       </c>
@@ -1703,7 +1695,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="47" t="s">
         <v>79</v>
       </c>
@@ -1729,7 +1721,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="47" t="s">
         <v>1</v>
       </c>
@@ -1754,7 +1746,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="47" t="s">
         <v>80</v>
       </c>
@@ -1780,7 +1772,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="14" t="s">
         <v>6</v>
       </c>
@@ -1804,7 +1796,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="52" t="s">
         <v>84</v>
       </c>
@@ -1828,7 +1820,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="48" t="s">
         <v>85</v>
       </c>
@@ -1854,14 +1846,14 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="27" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="10" t="s">
         <v>2</v>
       </c>
@@ -1872,7 +1864,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A28" s="46" t="s">
         <v>89</v>
       </c>
@@ -1883,7 +1875,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="47" t="s">
         <v>93</v>
       </c>
@@ -1894,33 +1886,33 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="B30" s="83">
+      <c r="B30" s="16">
         <v>2.6669999999999998</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B31" s="5"/>
       <c r="C31" s="4"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B32" s="5"/>
       <c r="C32" s="4"/>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="4"/>
       <c r="F33" s="5"/>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B34" s="4"/>
     </row>
   </sheetData>
@@ -1940,30 +1932,30 @@
   </sheetPr>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="11.875" customWidth="1"/>
+    <col min="4" max="7" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
@@ -1974,7 +1966,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A6" s="53" t="s">
         <v>95</v>
       </c>
@@ -1985,7 +1977,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="44" t="s">
         <v>96</v>
       </c>
@@ -1997,7 +1989,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="44" t="s">
         <v>97</v>
       </c>
@@ -2009,7 +2001,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="38" t="s">
         <v>20</v>
       </c>
@@ -2020,14 +2012,14 @@
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="10" t="s">
         <v>2</v>
       </c>
@@ -2038,32 +2030,32 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="84">
+      <c r="B15" s="28">
         <v>324.88600000000002</v>
       </c>
       <c r="C15" s="34" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A16" s="54"/>
       <c r="B16" s="6"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="54"/>
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="20" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="10" t="s">
         <v>2</v>
       </c>
@@ -2074,7 +2066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A21" s="36" t="s">
         <v>24</v>
       </c>
@@ -2083,7 +2075,7 @@
       </c>
       <c r="C21" s="31"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="37" t="s">
         <v>23</v>
       </c>
@@ -2093,7 +2085,7 @@
       <c r="C22" s="32"/>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="37" t="s">
         <v>27</v>
       </c>
@@ -2105,7 +2097,7 @@
       </c>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="37" t="s">
         <v>28</v>
       </c>
@@ -2116,7 +2108,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="37" t="s">
         <v>30</v>
       </c>
@@ -2127,7 +2119,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="38" t="s">
         <v>32</v>
       </c>
@@ -2138,14 +2130,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="31" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="10" t="s">
         <v>2</v>
       </c>
@@ -2168,7 +2160,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A32" s="36" t="s">
         <v>5</v>
       </c>
@@ -2191,7 +2183,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="58" t="s">
         <v>101</v>
       </c>
@@ -2201,20 +2193,20 @@
       <c r="C33" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="D33" s="85">
+      <c r="D33" s="55">
         <v>479.09</v>
       </c>
       <c r="E33" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="F33" s="85">
+      <c r="F33" s="55">
         <v>688.08799999999997</v>
       </c>
       <c r="G33" s="57" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="37" t="s">
         <v>15</v>
       </c>
@@ -2224,20 +2216,22 @@
       <c r="C34" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="D34" s="80">
-        <v>0.28727999999999998</v>
+      <c r="D34" s="83">
+        <f>SQRT(0.28728)</f>
+        <v>0.53598507441905507</v>
       </c>
       <c r="E34" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="F34" s="80">
-        <v>0.41413</v>
+      <c r="F34" s="83">
+        <f>SQRT(0.41413)</f>
+        <v>0.64352933111086708</v>
       </c>
       <c r="G34" s="26" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="38" t="s">
         <v>34</v>
       </c>
@@ -2247,27 +2241,29 @@
       <c r="C35" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="D35" s="81">
-        <v>10.728999999999999</v>
+      <c r="D35" s="84">
+        <f>D34^2*B25</f>
+        <v>37.346399999999996</v>
       </c>
       <c r="E35" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="F35" s="81">
-        <v>22.295000000000002</v>
+      <c r="F35" s="84">
+        <f>F34^2*B25</f>
+        <v>53.8369</v>
       </c>
       <c r="G35" s="30" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="38" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="40" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="10" t="s">
         <v>2</v>
       </c>
@@ -2278,7 +2274,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A41" s="53" t="s">
         <v>100</v>
       </c>
@@ -2289,7 +2285,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="58" t="s">
         <v>108</v>
       </c>
@@ -2301,40 +2297,40 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="44" t="s">
         <v>153</v>
       </c>
-      <c r="B43" s="82">
+      <c r="B43" s="85">
         <v>10</v>
       </c>
       <c r="C43" s="32" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="60" t="s">
         <v>154</v>
       </c>
-      <c r="B44" s="78">
+      <c r="B44" s="86">
         <v>14.33</v>
       </c>
       <c r="C44" s="32" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="B45" s="79">
+      <c r="B45" s="87">
         <v>214.95</v>
       </c>
       <c r="C45" s="34" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2346,28 +2342,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="7" width="11.875" customWidth="1"/>
+    <col min="2" max="7" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
@@ -2378,7 +2374,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A6" s="44" t="s">
         <v>175</v>
       </c>
@@ -2390,7 +2386,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="44" t="s">
         <v>111</v>
       </c>
@@ -2402,7 +2398,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="37" t="s">
         <v>112</v>
       </c>
@@ -2413,7 +2409,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="38" t="s">
         <v>114</v>
       </c>
@@ -2424,14 +2420,14 @@
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="10" t="s">
         <v>2</v>
       </c>
@@ -2442,7 +2438,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A15" s="36" t="s">
         <v>116</v>
       </c>
@@ -2451,7 +2447,7 @@
       </c>
       <c r="C15" s="23"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="44" t="s">
         <v>118</v>
       </c>
@@ -2462,7 +2458,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="37" t="s">
         <v>119</v>
       </c>
@@ -2473,7 +2469,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="37" t="s">
         <v>121</v>
       </c>
@@ -2484,7 +2480,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="37" t="s">
         <v>122</v>
       </c>
@@ -2495,7 +2491,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="37" t="s">
         <v>124</v>
       </c>
@@ -2507,7 +2503,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="37" t="s">
         <v>126</v>
       </c>
@@ -2519,7 +2515,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="38" t="s">
         <v>128</v>
       </c>
@@ -2528,23 +2524,23 @@
       </c>
       <c r="C22" s="34"/>
     </row>
-    <row r="23" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B23" s="5"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="72"/>
       <c r="B24" s="5"/>
     </row>
-    <row r="25" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>129</v>
       </c>
       <c r="B25" s="5"/>
     </row>
-    <row r="26" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="5"/>
     </row>
-    <row r="27" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="10" t="s">
         <v>2</v>
       </c>
@@ -2555,7 +2551,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A28" s="53" t="s">
         <v>130</v>
       </c>
@@ -2566,7 +2562,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="38" t="s">
         <v>131</v>
       </c>
@@ -2578,17 +2574,17 @@
       </c>
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B30" s="6"/>
       <c r="F30" s="7"/>
     </row>
-    <row r="32" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="34" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="10" t="s">
         <v>2</v>
       </c>
@@ -2599,7 +2595,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A35" s="58" t="s">
         <v>133</v>
       </c>
@@ -2610,18 +2606,18 @@
         <v>160</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="37" t="s">
         <v>134</v>
       </c>
       <c r="B36" s="27">
-        <v>0.29865999999999998</v>
+        <v>0.144708</v>
       </c>
       <c r="C36" s="32" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="44" t="s">
         <v>135</v>
       </c>
@@ -2632,22 +2628,22 @@
         <v>162</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="B38" s="86">
+      <c r="B38" s="27">
         <v>22.167000000000002</v>
       </c>
       <c r="C38" s="32" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="B39" s="86">
+      <c r="B39" s="27">
         <v>5.2374999999999998</v>
       </c>
       <c r="C39" s="32" t="s">
@@ -2655,25 +2651,25 @@
       </c>
       <c r="E39" s="73"/>
     </row>
-    <row r="40" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="B40" s="87">
+      <c r="B40" s="33">
         <v>145.03</v>
       </c>
       <c r="C40" s="34" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A43" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="45" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="10" t="s">
         <v>2</v>
       </c>
@@ -2696,7 +2692,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A46" s="36" t="s">
         <v>5</v>
       </c>
@@ -2719,46 +2715,46 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="B47" s="88">
+      <c r="B47" s="24">
         <v>1.29</v>
       </c>
       <c r="C47" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D47" s="88">
+      <c r="D47" s="24">
         <v>1.29</v>
       </c>
       <c r="E47" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F47" s="88">
+      <c r="F47" s="24">
         <v>1.29</v>
       </c>
       <c r="G47" s="26" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="B48" s="86">
+      <c r="B48" s="27">
         <v>241.34</v>
       </c>
       <c r="C48" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="D48" s="86">
+      <c r="D48" s="27">
         <v>241.34</v>
       </c>
       <c r="E48" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="F48" s="86">
+      <c r="F48" s="27">
         <v>241.34</v>
       </c>
       <c r="G48" s="26" t="s">
@@ -2777,28 +2773,28 @@
   </sheetPr>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.875" customWidth="1"/>
-    <col min="2" max="7" width="11.875" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="7" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
@@ -2809,7 +2805,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A6" s="36" t="s">
         <v>35</v>
       </c>
@@ -2821,7 +2817,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="37" t="s">
         <v>59</v>
       </c>
@@ -2833,7 +2829,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="38" t="s">
         <v>36</v>
       </c>
@@ -2844,14 +2840,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="10" t="s">
         <v>2</v>
       </c>
@@ -2862,7 +2858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A14" s="36" t="s">
         <v>24</v>
       </c>
@@ -2871,7 +2867,7 @@
       </c>
       <c r="C14" s="31"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="37" t="s">
         <v>39</v>
       </c>
@@ -2880,7 +2876,7 @@
       </c>
       <c r="C15" s="32"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="37" t="s">
         <v>40</v>
       </c>
@@ -2891,7 +2887,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="37" t="s">
         <v>41</v>
       </c>
@@ -2902,7 +2898,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="37" t="s">
         <v>42</v>
       </c>
@@ -2913,7 +2909,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="37" t="s">
         <v>43</v>
       </c>
@@ -2924,7 +2920,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="37" t="s">
         <v>45</v>
       </c>
@@ -2935,47 +2931,47 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="89">
+      <c r="B21" s="40">
         <v>4.5</v>
       </c>
       <c r="C21" s="32" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="89">
+      <c r="B22" s="40">
         <v>5</v>
       </c>
       <c r="C22" s="32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="90">
+      <c r="B23" s="41">
         <v>62</v>
       </c>
       <c r="C23" s="34" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="27" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="10" t="s">
         <v>2</v>
       </c>
@@ -2986,7 +2982,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A28" s="36" t="s">
         <v>53</v>
       </c>
@@ -2998,7 +2994,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="37" t="s">
         <v>54</v>
       </c>
@@ -3009,7 +3005,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="38" t="s">
         <v>52</v>
       </c>
@@ -3020,16 +3016,16 @@
         <v>166</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B31" s="6"/>
     </row>
-    <row r="33" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="35" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="10" t="s">
         <v>2</v>
       </c>
@@ -3052,7 +3048,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A36" s="36" t="s">
         <v>5</v>
       </c>
@@ -3075,7 +3071,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="44" t="s">
         <v>101</v>
       </c>
@@ -3101,7 +3097,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="37" t="s">
         <v>58</v>
       </c>
@@ -3126,7 +3122,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="37" t="s">
         <v>60</v>
       </c>
@@ -3136,14 +3132,14 @@
       <c r="C39" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="D39" s="86">
+      <c r="D39" s="27">
         <f>$B$7-((1*8*'Capacitor &amp; Controller'!$B$15*10^-6*D37)/2)</f>
         <v>0.66440146503999986</v>
       </c>
       <c r="E39" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="F39" s="86">
+      <c r="F39" s="27">
         <f>$B$7-((1*8*'Capacitor &amp; Controller'!$B$15*10^-6*F37)/2)</f>
         <v>0.39279936812799987</v>
       </c>
@@ -3151,7 +3147,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="37" t="s">
         <v>61</v>
       </c>
@@ -3161,14 +3157,14 @@
       <c r="C40" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="D40" s="86">
+      <c r="D40" s="27">
         <f>$B$7+((1*8*'Capacitor &amp; Controller'!$B$15*10^-6*D37)/2)</f>
         <v>1.90959853496</v>
       </c>
       <c r="E40" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="F40" s="86">
+      <c r="F40" s="27">
         <f>$B$7+((1*8*'Capacitor &amp; Controller'!$B$15*10^-6*F37)/2)</f>
         <v>2.1812006318720001</v>
       </c>
@@ -3176,25 +3172,25 @@
         <v>167</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="B41" s="86">
+      <c r="B41" s="27">
         <f>($B$6-$B$22*10^-3*B39)*(($B$30*$B$20*10^-12)/($B$28-$B$21))*10^9</f>
         <v>10.071428571428571</v>
       </c>
       <c r="C41" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="D41" s="86">
+      <c r="D41" s="27">
         <f>($B$6-$B$22*10^-3*D39)*(($B$30*$B$20*10^-12)/($B$28-$B$21))*10^9</f>
         <v>10.069198080795937</v>
       </c>
       <c r="E41" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="F41" s="86">
+      <c r="F41" s="27">
         <f>($B$6-$B$22*10^-3*F39)*(($B$30*$B$20*10^-12)/($B$28-$B$21))*10^9</f>
         <v>10.070109887835573</v>
       </c>
@@ -3202,25 +3198,25 @@
         <v>168</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="86">
+      <c r="B42" s="27">
         <f>($B$6-$B$22*10^-3*$D$40)*(($B$30*$B$20*10^-12)/($B$21))*10^9</f>
         <v>23.485041478142811</v>
       </c>
       <c r="C42" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="D42" s="86">
+      <c r="D42" s="27">
         <f>($B$6-$B$22*10^-3*$D$40)*(($B$30*$B$20*10^-12)/($B$21))*10^9</f>
         <v>23.485041478142811</v>
       </c>
       <c r="E42" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F42" s="86">
+      <c r="F42" s="27">
         <f>($B$6-$B$22*10^-3*$D$40)*(($B$30*$B$20*10^-12)/($B$21))*10^9</f>
         <v>23.485041478142811</v>
       </c>
@@ -3228,25 +3224,25 @@
         <v>143</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="B43" s="86">
+      <c r="B43" s="27">
         <f>$B$18+$B$41</f>
         <v>15.071428571428571</v>
       </c>
       <c r="C43" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="D43" s="86">
+      <c r="D43" s="27">
         <f>$B$18+$B$41</f>
         <v>15.071428571428571</v>
       </c>
       <c r="E43" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="F43" s="86">
+      <c r="F43" s="27">
         <f>$B$18+$B$41</f>
         <v>15.071428571428571</v>
       </c>
@@ -3254,25 +3250,25 @@
         <v>144</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="B44" s="86">
+      <c r="B44" s="27">
         <f>$B$19+$B$42</f>
         <v>35.485041478142811</v>
       </c>
       <c r="C44" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="D44" s="86">
+      <c r="D44" s="27">
         <f>$B$19+$B$42</f>
         <v>35.485041478142811</v>
       </c>
       <c r="E44" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="F44" s="86">
+      <c r="F44" s="27">
         <f>$B$19+$B$42</f>
         <v>35.485041478142811</v>
       </c>
@@ -3280,24 +3276,24 @@
         <v>145</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="B45" s="86">
+      <c r="B45" s="27">
         <v>0</v>
       </c>
       <c r="C45" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="D45" s="86">
+      <c r="D45" s="27">
         <f>((D37*$B$6)/2)*(D39*D43*10^-9+D40*D44*10^-9)*1000</f>
         <v>0.27946156589776133</v>
       </c>
       <c r="E45" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="F45" s="86">
+      <c r="F45" s="27">
         <f>((F37*$B$6)/2)*(F39*F43*10^-9+F40*F44*10^-9)*1000</f>
         <v>0.42998641059912607</v>
       </c>
@@ -3305,24 +3301,24 @@
         <v>169</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="B46" s="86">
+      <c r="B46" s="27">
         <v>0</v>
       </c>
       <c r="C46" s="29" t="s">
         <v>170</v>
       </c>
-      <c r="D46" s="86">
+      <c r="D46" s="27">
         <f>D$38^2*$B$22</f>
         <v>1.8468514349999996</v>
       </c>
       <c r="E46" s="29" t="s">
         <v>170</v>
       </c>
-      <c r="F46" s="86">
+      <c r="F46" s="27">
         <f>F$38^2*$B$22</f>
         <v>4.4208488610000005</v>
       </c>
@@ -3330,24 +3326,24 @@
         <v>170</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B47" s="84">
+      <c r="B47" s="28">
         <v>0</v>
       </c>
       <c r="C47" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="D47" s="84">
+      <c r="D47" s="28">
         <f>SUM(D45:D46)</f>
         <v>2.1263130008977611</v>
       </c>
       <c r="E47" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="F47" s="84">
+      <c r="F47" s="28">
         <f>SUM(F45:F46)</f>
         <v>4.8508352715991263</v>
       </c>
@@ -3355,14 +3351,14 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="50" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A50" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="52" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="10" t="s">
         <v>2</v>
       </c>
@@ -3373,11 +3369,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="B53" s="91">
+      <c r="B53" s="78">
         <f>B8+B23*F47*10^-3</f>
         <v>30.300751786839147</v>
       </c>
@@ -3385,7 +3381,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3400,28 +3396,28 @@
   </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.25" customWidth="1"/>
-    <col min="2" max="7" width="11.875" customWidth="1"/>
+    <col min="2" max="7" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
@@ -3432,7 +3428,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A6" s="36" t="s">
         <v>66</v>
       </c>
@@ -3444,7 +3440,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="37" t="s">
         <v>67</v>
       </c>
@@ -3456,7 +3452,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="38" t="s">
         <v>36</v>
       </c>
@@ -3467,14 +3463,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="10" t="s">
         <v>2</v>
       </c>
@@ -3485,7 +3481,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A14" s="36" t="s">
         <v>24</v>
       </c>
@@ -3494,16 +3490,16 @@
       </c>
       <c r="C14" s="31"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="92" t="s">
+      <c r="B15" s="81" t="s">
         <v>180</v>
       </c>
-      <c r="C15" s="93"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" s="82"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="37" t="s">
         <v>69</v>
       </c>
@@ -3514,18 +3510,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="89">
+      <c r="B17" s="40">
         <v>10</v>
       </c>
       <c r="C17" s="26" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="37" t="s">
         <v>71</v>
       </c>
@@ -3536,25 +3532,25 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="94" t="s">
+      <c r="B19" s="79" t="s">
         <v>181</v>
       </c>
       <c r="C19" s="34" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="24" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="10" t="s">
         <v>2</v>
       </c>
@@ -3577,7 +3573,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A25" s="36" t="s">
         <v>5</v>
       </c>
@@ -3600,7 +3596,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="37" t="s">
         <v>6</v>
       </c>
@@ -3626,25 +3622,25 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="86">
+      <c r="B27" s="27">
         <f>B7</f>
         <v>1.2869999999999999</v>
       </c>
       <c r="C27" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="D27" s="86">
+      <c r="D27" s="27">
         <f>(1-D26/100)*$B$7</f>
         <v>0.99999899999999997</v>
       </c>
       <c r="E27" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="F27" s="86">
+      <c r="F27" s="27">
         <f>(1-F26/100)*$B$7</f>
         <v>0.59999939999999985</v>
       </c>
@@ -3652,25 +3648,25 @@
         <v>172</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="86">
+      <c r="B28" s="27">
         <f>(1-B26/100)*$B$18*$B$7</f>
         <v>0.73358999999999985</v>
       </c>
       <c r="C28" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="D28" s="86">
+      <c r="D28" s="27">
         <f>(1-D26/100)*$B$18*$B$7</f>
         <v>0.56999942999999986</v>
       </c>
       <c r="E28" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="F28" s="86">
+      <c r="F28" s="27">
         <f>(1-F26/100)*$B$18*$B$7</f>
         <v>0.34199965799999993</v>
       </c>
@@ -3678,48 +3674,48 @@
         <v>173</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="B29" s="86">
+      <c r="B29" s="27">
         <v>0</v>
       </c>
       <c r="C29" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="D29" s="86">
+      <c r="D29" s="27">
         <v>0</v>
       </c>
       <c r="E29" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="F29" s="86">
+      <c r="F29" s="27">
         <v>0</v>
       </c>
       <c r="G29" s="25" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="84">
+      <c r="B30" s="28">
         <f>SUM(B28:B29)</f>
         <v>0.73358999999999985</v>
       </c>
       <c r="C30" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="D30" s="84">
+      <c r="D30" s="28">
         <f>SUM(D28:D29)</f>
         <v>0.56999942999999986</v>
       </c>
       <c r="E30" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="F30" s="84">
+      <c r="F30" s="28">
         <f>SUM(F28:F29)</f>
         <v>0.34199965799999993</v>
       </c>
@@ -3727,14 +3723,14 @@
         <v>148</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="35" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="10" t="s">
         <v>2</v>
       </c>
@@ -3745,24 +3741,24 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="91">
+      <c r="B36" s="78">
         <v>75</v>
       </c>
       <c r="C36" s="42" t="s">
         <v>174</v>
       </c>
-      <c r="D36" s="95" t="s">
+      <c r="D36" s="80" t="s">
         <v>182</v>
       </c>
-      <c r="E36" s="95"/>
-      <c r="F36" s="95"/>
-      <c r="G36" s="95"/>
-    </row>
-    <row r="37" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="E36" s="80"/>
+      <c r="F36" s="80"/>
+      <c r="G36" s="80"/>
+    </row>
+    <row r="37" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B15:C15"/>

</xml_diff>